<commit_message>
Updated the rubric to track completed objectives so far
</commit_message>
<xml_diff>
--- a/Paperwork/Project Rubric.xlsx
+++ b/Paperwork/Project Rubric.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Qsync\Graphics I &amp; II Shared Staff Folder\Project &amp; Portfolio IV\Week_2_Handout\Assignments\The Level Renderer\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Full Sail University\Project Portfolio 4 V2\LevelRenderer\Paperwork\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A67AA71-4396-459B-8D32-559B140E8793}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{991E1F96-2C39-4072-8586-7CDA4C8035CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7485" yWindow="0" windowWidth="35145" windowHeight="17280" xr2:uid="{2B9022D0-B5E6-432E-8A19-30BD25892E64}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2B9022D0-B5E6-432E-8A19-30BD25892E64}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1267,7 +1267,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="50">
   <si>
     <t>1. One or More Blender Game Levels to export from (.blend)</t>
   </si>
@@ -1414,6 +1414,9 @@
   </si>
   <si>
     <t>Make the camera Collide with your Level</t>
+  </si>
+  <si>
+    <t>*</t>
   </si>
 </sst>
 </file>
@@ -2028,10 +2031,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4A40538-A3BB-461B-BC01-A04BD38DD6FA}">
-  <dimension ref="A1:C50"/>
+  <dimension ref="A1:D50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="D46" sqref="D46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2040,7 +2043,7 @@
     <col min="2" max="3" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>27</v>
       </c>
@@ -2051,7 +2054,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -2061,8 +2064,11 @@
       <c r="C2" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -2072,8 +2078,11 @@
       <c r="C3" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>36</v>
       </c>
@@ -2083,8 +2092,11 @@
       <c r="C4" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>37</v>
       </c>
@@ -2095,7 +2107,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>2</v>
       </c>
@@ -2106,7 +2118,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>25</v>
       </c>
@@ -2117,7 +2129,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>42</v>
       </c>
@@ -2128,7 +2140,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>43</v>
       </c>
@@ -2139,7 +2151,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>44</v>
       </c>
@@ -2150,7 +2162,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>24</v>
       </c>
@@ -2161,7 +2173,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>4</v>
       </c>
@@ -2174,7 +2186,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>6</v>
       </c>
@@ -2185,7 +2197,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
         <v>22</v>
       </c>
@@ -2196,7 +2208,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
         <v>41</v>
       </c>
@@ -2207,7 +2219,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
         <v>40</v>
       </c>
@@ -2395,7 +2407,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="8" t="s">
         <v>35</v>
       </c>
@@ -2406,7 +2418,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="18" t="s">
         <v>16</v>
       </c>
@@ -2417,7 +2429,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="18" t="s">
         <v>32</v>
       </c>
@@ -2428,7 +2440,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="18" t="s">
         <v>17</v>
       </c>
@@ -2439,7 +2451,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="18" t="s">
         <v>38</v>
       </c>
@@ -2450,7 +2462,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="18" t="s">
         <v>18</v>
       </c>
@@ -2461,7 +2473,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="18" t="s">
         <v>19</v>
       </c>
@@ -2472,7 +2484,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="18" t="s">
         <v>31</v>
       </c>
@@ -2483,7 +2495,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="18" t="s">
         <v>33</v>
       </c>
@@ -2494,7 +2506,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="18" t="s">
         <v>39</v>
       </c>
@@ -2505,7 +2517,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="11" t="s">
         <v>15</v>
       </c>
@@ -2516,7 +2528,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
         <v>4</v>
       </c>
@@ -2528,7 +2540,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:3" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A45" s="1" t="s">
         <v>29</v>
       </c>
@@ -2539,7 +2551,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="46" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
         <v>46</v>
       </c>
@@ -2550,7 +2562,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
         <v>28</v>
       </c>
@@ -2560,8 +2572,11 @@
       <c r="C47" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="48" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D47" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="12" t="s">
         <v>45</v>
       </c>

</xml_diff>

<commit_message>
Updated rubric to accurately represent progress
</commit_message>
<xml_diff>
--- a/Paperwork/Project Rubric.xlsx
+++ b/Paperwork/Project Rubric.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Full Sail University\Project Portfolio 4 V2\LevelRenderer\Paperwork\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{991E1F96-2C39-4072-8586-7CDA4C8035CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EB80CB2-DBA7-48FF-834F-EFD9FDEDE363}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2B9022D0-B5E6-432E-8A19-30BD25892E64}"/>
   </bookViews>
@@ -1267,7 +1267,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="50">
   <si>
     <t>1. One or More Blender Game Levels to export from (.blend)</t>
   </si>
@@ -2033,8 +2033,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4A40538-A3BB-461B-BC01-A04BD38DD6FA}">
   <dimension ref="A1:D50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="D46" sqref="D46"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2106,6 +2106,9 @@
       <c r="C5" s="3">
         <v>0</v>
       </c>
+      <c r="D5" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
@@ -2117,6 +2120,9 @@
       <c r="C6" s="3">
         <v>0</v>
       </c>
+      <c r="D6" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
@@ -2128,6 +2134,9 @@
       <c r="C7" s="3">
         <v>0</v>
       </c>
+      <c r="D7" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
@@ -2139,6 +2148,9 @@
       <c r="C8" s="3">
         <v>0</v>
       </c>
+      <c r="D8" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
@@ -2150,6 +2162,9 @@
       <c r="C9" s="3">
         <v>0</v>
       </c>
+      <c r="D9" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
@@ -2171,6 +2186,9 @@
       </c>
       <c r="C11" s="3">
         <v>0</v>
+      </c>
+      <c r="D11" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Fixed Models and added Point Light from Blender
</commit_message>
<xml_diff>
--- a/Paperwork/Project Rubric.xlsx
+++ b/Paperwork/Project Rubric.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Full Sail University\Project Portfolio 4 V2\LevelRenderer\Paperwork\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EB80CB2-DBA7-48FF-834F-EFD9FDEDE363}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBB640B3-815D-452D-BAA6-C48F358A612F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2B9022D0-B5E6-432E-8A19-30BD25892E64}"/>
   </bookViews>
@@ -1267,7 +1267,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="50">
   <si>
     <t>1. One or More Blender Game Levels to export from (.blend)</t>
   </si>
@@ -2033,8 +2033,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4A40538-A3BB-461B-BC01-A04BD38DD6FA}">
   <dimension ref="A1:D50"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2176,6 +2176,9 @@
       <c r="C10" s="3">
         <v>0</v>
       </c>
+      <c r="D10" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">

</xml_diff>

<commit_message>
Updated Rubric to show proper progress
</commit_message>
<xml_diff>
--- a/Paperwork/Project Rubric.xlsx
+++ b/Paperwork/Project Rubric.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Full Sail University\Project Portfolio 4 V2\LevelRenderer\Paperwork\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBB640B3-815D-452D-BAA6-C48F358A612F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF99329D-236D-4B40-80A5-AF8930099783}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2B9022D0-B5E6-432E-8A19-30BD25892E64}"/>
   </bookViews>
@@ -1267,7 +1267,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="50">
   <si>
     <t>1. One or More Blender Game Levels to export from (.blend)</t>
   </si>
@@ -2033,8 +2033,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4A40538-A3BB-461B-BC01-A04BD38DD6FA}">
   <dimension ref="A1:D50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2228,6 +2228,9 @@
       <c r="C14" s="3">
         <v>0</v>
       </c>
+      <c r="D14" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">

</xml_diff>